<commit_message>
cleveland clinic answer import preliminary version
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-answers.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-answers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -102,9 +102,6 @@
     <t>answer_exercise_benchpress</t>
   </si>
   <si>
-    <t>answer_exercise_longjump</t>
-  </si>
-  <si>
     <t>exercise_key</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>television_key</t>
+  </si>
+  <si>
+    <t>answer_exercise_longjump_feet</t>
+  </si>
+  <si>
+    <t>answer_exercise_longjump_inches</t>
   </si>
 </sst>
 </file>
@@ -721,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1085,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>8</v>
@@ -1111,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>8</v>
@@ -1137,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>8</v>
@@ -1163,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>8</v>
@@ -1189,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2">
         <v>250</v>
@@ -1209,13 +1212,13 @@
         <v>28</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E19" s="2">
         <v>7</v>
@@ -1235,13 +1238,13 @@
         <v>29</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E20" s="2">
         <v>6</v>
@@ -1261,13 +1264,13 @@
         <v>30</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>8</v>
@@ -1287,13 +1290,13 @@
         <v>31</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>8</v>
@@ -1313,13 +1316,13 @@
         <v>32</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>8</v>
@@ -1339,13 +1342,13 @@
         <v>33</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>8</v>
@@ -1365,13 +1368,13 @@
         <v>34</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>8</v>
@@ -1391,13 +1394,13 @@
         <v>35</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C26" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>8</v>
@@ -1735,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>8</v>
@@ -1761,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>8</v>
@@ -1787,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>8</v>
@@ -1813,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>8</v>
@@ -1839,7 +1842,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E43" s="2">
         <v>255</v>
@@ -1859,13 +1862,13 @@
         <v>54</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E44" s="2">
         <v>7</v>
@@ -1885,13 +1888,13 @@
         <v>55</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E45" s="2">
         <v>8</v>
@@ -1911,13 +1914,13 @@
         <v>56</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>8</v>
@@ -1937,13 +1940,13 @@
         <v>57</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>8</v>
@@ -1963,13 +1966,13 @@
         <v>58</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>8</v>
@@ -1989,13 +1992,13 @@
         <v>59</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>8</v>
@@ -2015,13 +2018,13 @@
         <v>60</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C50" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>8</v>
@@ -2041,13 +2044,13 @@
         <v>61</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C51" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>8</v>
@@ -2385,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>8</v>
@@ -2411,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>8</v>
@@ -2437,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>8</v>
@@ -2463,7 +2466,7 @@
         <v>0</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>8</v>
@@ -2489,7 +2492,7 @@
         <v>8</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E68" s="2">
         <v>255</v>
@@ -2509,13 +2512,13 @@
         <v>79</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E69" s="2">
         <v>7</v>
@@ -2535,13 +2538,13 @@
         <v>80</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E70" s="2">
         <v>8</v>
@@ -2561,13 +2564,13 @@
         <v>81</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C71" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>8</v>
@@ -2587,13 +2590,13 @@
         <v>82</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C72" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>8</v>
@@ -2613,13 +2616,13 @@
         <v>83</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C73" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>8</v>
@@ -2639,13 +2642,13 @@
         <v>84</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>8</v>
@@ -2665,13 +2668,13 @@
         <v>85</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C75" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>8</v>
@@ -2691,13 +2694,13 @@
         <v>86</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
ccf import/export multiple user test
</commit_message>
<xml_diff>
--- a/api/test/fixtures/import-export/ccf/ccf-answers.xlsx
+++ b/api/test/fixtures/import-export/ccf/ccf-answers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="1380" windowWidth="25600" windowHeight="13240"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -192,8 +192,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -264,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -295,6 +309,13 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -325,6 +346,13 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2715,6 +2743,1956 @@
         <v>1</v>
       </c>
     </row>
+    <row r="77" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A77" s="1">
+        <v>88</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="2">
+        <v>20852</v>
+      </c>
+      <c r="F77" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G77" s="1">
+        <v>87</v>
+      </c>
+      <c r="H77" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A78" s="1">
+        <v>89</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="2">
+        <v>3</v>
+      </c>
+      <c r="F78" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G78" s="1">
+        <v>87</v>
+      </c>
+      <c r="H78" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A79" s="1">
+        <v>90</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="2">
+        <v>16</v>
+      </c>
+      <c r="F79" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G79" s="1">
+        <v>87</v>
+      </c>
+      <c r="H79" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A80" s="1">
+        <v>91</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="2">
+        <v>1990</v>
+      </c>
+      <c r="F80" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G80" s="1">
+        <v>87</v>
+      </c>
+      <c r="H80" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A81" s="1">
+        <v>92</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G81" s="1">
+        <v>87</v>
+      </c>
+      <c r="H81" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A82" s="1">
+        <v>93</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G82" s="1">
+        <v>87</v>
+      </c>
+      <c r="H82" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A83" s="1">
+        <v>94</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G83" s="1">
+        <v>87</v>
+      </c>
+      <c r="H83" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A84" s="1">
+        <v>95</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G84" s="1">
+        <v>87</v>
+      </c>
+      <c r="H84" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A85" s="1">
+        <v>96</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G85" s="1">
+        <v>87</v>
+      </c>
+      <c r="H85" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A86" s="1">
+        <v>97</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G86" s="1">
+        <v>87</v>
+      </c>
+      <c r="H86" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A87" s="1">
+        <v>98</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G87" s="1">
+        <v>87</v>
+      </c>
+      <c r="H87" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A88" s="1">
+        <v>99</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G88" s="1">
+        <v>87</v>
+      </c>
+      <c r="H88" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A89" s="1">
+        <v>100</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" s="3">
+        <v>42669.030266203707</v>
+      </c>
+      <c r="G89" s="1">
+        <v>87</v>
+      </c>
+      <c r="H89" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A90" s="1">
+        <v>101</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" s="3">
+        <v>42669.030266203707</v>
+      </c>
+      <c r="G90" s="1">
+        <v>87</v>
+      </c>
+      <c r="H90" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A91" s="1">
+        <v>102</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" s="3">
+        <v>42669.030266203707</v>
+      </c>
+      <c r="G91" s="1">
+        <v>87</v>
+      </c>
+      <c r="H91" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A92" s="1">
+        <v>103</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" s="3">
+        <v>42669.030266203707</v>
+      </c>
+      <c r="G92" s="1">
+        <v>87</v>
+      </c>
+      <c r="H92" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A93" s="1">
+        <v>104</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E93" s="2">
+        <v>244</v>
+      </c>
+      <c r="F93" s="3">
+        <v>42669.030266203707</v>
+      </c>
+      <c r="G93" s="1">
+        <v>87</v>
+      </c>
+      <c r="H93" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A94" s="1">
+        <v>105</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E94" s="2">
+        <v>7</v>
+      </c>
+      <c r="F94" s="3">
+        <v>42669.030266203707</v>
+      </c>
+      <c r="G94" s="1">
+        <v>87</v>
+      </c>
+      <c r="H94" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A95" s="1">
+        <v>106</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" s="2">
+        <v>5</v>
+      </c>
+      <c r="F95" s="3">
+        <v>42669.030266203707</v>
+      </c>
+      <c r="G95" s="1">
+        <v>87</v>
+      </c>
+      <c r="H95" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A96" s="1">
+        <v>107</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="3">
+        <v>42669.030694444446</v>
+      </c>
+      <c r="G96" s="1">
+        <v>87</v>
+      </c>
+      <c r="H96" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A97" s="1">
+        <v>108</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F97" s="3">
+        <v>42669.030694444446</v>
+      </c>
+      <c r="G97" s="1">
+        <v>87</v>
+      </c>
+      <c r="H97" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A98" s="1">
+        <v>109</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" s="3">
+        <v>42669.030694444446</v>
+      </c>
+      <c r="G98" s="1">
+        <v>87</v>
+      </c>
+      <c r="H98" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A99" s="1">
+        <v>110</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="3">
+        <v>42669.030694444446</v>
+      </c>
+      <c r="G99" s="1">
+        <v>87</v>
+      </c>
+      <c r="H99" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A100" s="1">
+        <v>111</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F100" s="3">
+        <v>42669.030694444446</v>
+      </c>
+      <c r="G100" s="1">
+        <v>87</v>
+      </c>
+      <c r="H100" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A101" s="1">
+        <v>112</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" s="3">
+        <v>42669.030694444446</v>
+      </c>
+      <c r="G101" s="1">
+        <v>87</v>
+      </c>
+      <c r="H101" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A102" s="1">
+        <v>114</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="2">
+        <v>20852</v>
+      </c>
+      <c r="F102" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G102" s="1">
+        <v>113</v>
+      </c>
+      <c r="H102" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A103" s="1">
+        <v>115</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="2">
+        <v>3</v>
+      </c>
+      <c r="F103" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G103" s="1">
+        <v>113</v>
+      </c>
+      <c r="H103" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A104" s="1">
+        <v>116</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="2">
+        <v>16</v>
+      </c>
+      <c r="F104" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G104" s="1">
+        <v>113</v>
+      </c>
+      <c r="H104" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A105" s="1">
+        <v>117</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="2">
+        <v>1990</v>
+      </c>
+      <c r="F105" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G105" s="1">
+        <v>113</v>
+      </c>
+      <c r="H105" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A106" s="1">
+        <v>118</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G106" s="1">
+        <v>113</v>
+      </c>
+      <c r="H106" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A107" s="1">
+        <v>119</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G107" s="1">
+        <v>113</v>
+      </c>
+      <c r="H107" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A108" s="1">
+        <v>120</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G108" s="1">
+        <v>113</v>
+      </c>
+      <c r="H108" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A109" s="1">
+        <v>121</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G109" s="1">
+        <v>113</v>
+      </c>
+      <c r="H109" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A110" s="1">
+        <v>122</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G110" s="1">
+        <v>113</v>
+      </c>
+      <c r="H110" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A111" s="1">
+        <v>123</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G111" s="1">
+        <v>113</v>
+      </c>
+      <c r="H111" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A112" s="1">
+        <v>124</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C112" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G112" s="1">
+        <v>113</v>
+      </c>
+      <c r="H112" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A113" s="1">
+        <v>125</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G113" s="1">
+        <v>113</v>
+      </c>
+      <c r="H113" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A114" s="1">
+        <v>126</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G114" s="1">
+        <v>113</v>
+      </c>
+      <c r="H114" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A115" s="1">
+        <v>127</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F115" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G115" s="1">
+        <v>113</v>
+      </c>
+      <c r="H115" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A116" s="1">
+        <v>128</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G116" s="1">
+        <v>113</v>
+      </c>
+      <c r="H116" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A117" s="1">
+        <v>129</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G117" s="1">
+        <v>113</v>
+      </c>
+      <c r="H117" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A118" s="1">
+        <v>130</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E118" s="2">
+        <v>250</v>
+      </c>
+      <c r="F118" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G118" s="1">
+        <v>113</v>
+      </c>
+      <c r="H118" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A119" s="1">
+        <v>131</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E119" s="2">
+        <v>7</v>
+      </c>
+      <c r="F119" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G119" s="1">
+        <v>113</v>
+      </c>
+      <c r="H119" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A120" s="1">
+        <v>132</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E120" s="2">
+        <v>9</v>
+      </c>
+      <c r="F120" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G120" s="1">
+        <v>113</v>
+      </c>
+      <c r="H120" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A121" s="1">
+        <v>133</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F121" s="6">
+        <v>42682.546006944445</v>
+      </c>
+      <c r="G121" s="1">
+        <v>113</v>
+      </c>
+      <c r="H121" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A122" s="1">
+        <v>134</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C122" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F122" s="6">
+        <v>42682.546006944445</v>
+      </c>
+      <c r="G122" s="1">
+        <v>113</v>
+      </c>
+      <c r="H122" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A123" s="1">
+        <v>135</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C123" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F123" s="6">
+        <v>42682.546006944445</v>
+      </c>
+      <c r="G123" s="1">
+        <v>113</v>
+      </c>
+      <c r="H123" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A124" s="1">
+        <v>136</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C124" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F124" s="6">
+        <v>42682.546006944445</v>
+      </c>
+      <c r="G124" s="1">
+        <v>113</v>
+      </c>
+      <c r="H124" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A125" s="1">
+        <v>137</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C125" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F125" s="6">
+        <v>42682.546006944445</v>
+      </c>
+      <c r="G125" s="1">
+        <v>113</v>
+      </c>
+      <c r="H125" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A126" s="1">
+        <v>138</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C126" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="6">
+        <v>42682.546006944445</v>
+      </c>
+      <c r="G126" s="1">
+        <v>113</v>
+      </c>
+      <c r="H126" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A127" s="1">
+        <v>140</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" s="2">
+        <v>20852</v>
+      </c>
+      <c r="F127" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G127" s="1">
+        <v>139</v>
+      </c>
+      <c r="H127" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A128" s="1">
+        <v>141</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="2">
+        <v>3</v>
+      </c>
+      <c r="F128" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G128" s="1">
+        <v>139</v>
+      </c>
+      <c r="H128" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A129" s="1">
+        <v>142</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="2">
+        <v>16</v>
+      </c>
+      <c r="F129" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G129" s="1">
+        <v>139</v>
+      </c>
+      <c r="H129" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A130" s="1">
+        <v>143</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" s="2">
+        <v>1990</v>
+      </c>
+      <c r="F130" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G130" s="1">
+        <v>139</v>
+      </c>
+      <c r="H130" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A131" s="1">
+        <v>144</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C131" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F131" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G131" s="1">
+        <v>139</v>
+      </c>
+      <c r="H131" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A132" s="1">
+        <v>145</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F132" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G132" s="1">
+        <v>139</v>
+      </c>
+      <c r="H132" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A133" s="1">
+        <v>146</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C133" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G133" s="1">
+        <v>139</v>
+      </c>
+      <c r="H133" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A134" s="1">
+        <v>147</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C134" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G134" s="1">
+        <v>139</v>
+      </c>
+      <c r="H134" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A135" s="1">
+        <v>148</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C135" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F135" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G135" s="1">
+        <v>139</v>
+      </c>
+      <c r="H135" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A136" s="1">
+        <v>149</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C136" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F136" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G136" s="1">
+        <v>139</v>
+      </c>
+      <c r="H136" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A137" s="1">
+        <v>150</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F137" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G137" s="1">
+        <v>139</v>
+      </c>
+      <c r="H137" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A138" s="1">
+        <v>151</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C138" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F138" s="6">
+        <v>42667.840555555558</v>
+      </c>
+      <c r="G138" s="1">
+        <v>139</v>
+      </c>
+      <c r="H138" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A139" s="1">
+        <v>152</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C139" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F139" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G139" s="1">
+        <v>139</v>
+      </c>
+      <c r="H139" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A140" s="1">
+        <v>153</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C140" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F140" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G140" s="1">
+        <v>139</v>
+      </c>
+      <c r="H140" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A141" s="1">
+        <v>154</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F141" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G141" s="1">
+        <v>139</v>
+      </c>
+      <c r="H141" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A142" s="1">
+        <v>155</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C142" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G142" s="1">
+        <v>139</v>
+      </c>
+      <c r="H142" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A143" s="1">
+        <v>156</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E143" s="2">
+        <v>250</v>
+      </c>
+      <c r="F143" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G143" s="1">
+        <v>139</v>
+      </c>
+      <c r="H143" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A144" s="1">
+        <v>157</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E144" s="2">
+        <v>7</v>
+      </c>
+      <c r="F144" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G144" s="1">
+        <v>139</v>
+      </c>
+      <c r="H144" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A145" s="1">
+        <v>158</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E145" s="2">
+        <v>9</v>
+      </c>
+      <c r="F145" s="6">
+        <v>42682.545659722222</v>
+      </c>
+      <c r="G145" s="1">
+        <v>139</v>
+      </c>
+      <c r="H145" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A146" s="1">
+        <v>158</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C146" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F146" s="6">
+        <v>42712.627893518518</v>
+      </c>
+      <c r="G146" s="1">
+        <v>139</v>
+      </c>
+      <c r="H146" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A147" s="1">
+        <v>159</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C147" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F147" s="6">
+        <v>42712.627893518518</v>
+      </c>
+      <c r="G147" s="1">
+        <v>139</v>
+      </c>
+      <c r="H147" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A148" s="1">
+        <v>160</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C148" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F148" s="6">
+        <v>42712.627893518518</v>
+      </c>
+      <c r="G148" s="1">
+        <v>139</v>
+      </c>
+      <c r="H148" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A149" s="1">
+        <v>161</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C149" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F149" s="6">
+        <v>42712.627893518518</v>
+      </c>
+      <c r="G149" s="1">
+        <v>139</v>
+      </c>
+      <c r="H149" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A150" s="1">
+        <v>162</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C150" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F150" s="6">
+        <v>42712.627893518518</v>
+      </c>
+      <c r="G150" s="1">
+        <v>139</v>
+      </c>
+      <c r="H150" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A151" s="1">
+        <v>163</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C151" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F151" s="6">
+        <v>42712.627893518518</v>
+      </c>
+      <c r="G151" s="1">
+        <v>139</v>
+      </c>
+      <c r="H151" s="1">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>